<commit_message>
update odds data, modelling
</commit_message>
<xml_diff>
--- a/group_stage_betting_odds.xlsx
+++ b/group_stage_betting_odds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Documents\GitHub\15095-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC9756A-813F-43C1-A475-71D3ABDC3124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D70855-A569-4791-AC1B-D3701369C041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5148" yWindow="732" windowWidth="15552" windowHeight="8904" xr2:uid="{3A73DD24-DA5B-4C59-823B-E318CD97E5CB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{3A73DD24-DA5B-4C59-823B-E318CD97E5CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
   <si>
     <t>Senegal</t>
   </si>
@@ -137,22 +137,28 @@
     <t>South Korea</t>
   </si>
   <si>
-    <t>betting team</t>
-  </si>
-  <si>
-    <t>challenger</t>
-  </si>
-  <si>
-    <t>earnings_on_100</t>
-  </si>
-  <si>
     <t>decimal_odds</t>
   </si>
   <si>
-    <t>american_odds</t>
-  </si>
-  <si>
     <t>implied_probability_of_win</t>
+  </si>
+  <si>
+    <t>home_team</t>
+  </si>
+  <si>
+    <t>away_team</t>
+  </si>
+  <si>
+    <t>home_earnings_on_100</t>
+  </si>
+  <si>
+    <t>away_earnings_on_100</t>
+  </si>
+  <si>
+    <t>home_american_odds</t>
+  </si>
+  <si>
+    <t>away_american_odds</t>
   </si>
 </sst>
 </file>
@@ -514,43 +520,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422B0D2D-1841-4969-922B-B7B831847234}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.20703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -560,20 +574,24 @@
       <c r="C2">
         <v>150</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <f>IF($C2&gt;0,$C2/100,(100)/(-$C2)+1)</f>
         <v>1.5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>IF($C2&gt;0,$C2,(100)/(-$C2)*100)</f>
         <v>150</v>
       </c>
-      <c r="F2" s="2">
-        <f>(1/D2)</f>
+      <c r="G2" s="2" t="e">
+        <f>IF($D2&gt;0,$D2,(100)/(-$D2)*100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2" s="2">
+        <f>(1/E2)</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -581,22 +599,29 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <v>125</v>
-      </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:D49" si="0">IF($C3&gt;0,$C3/100,(100)/(-$C3)+1)</f>
-        <v>1.25</v>
+        <v>400</v>
+      </c>
+      <c r="D3">
+        <v>-135</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E49" si="1">IF($C3&gt;0,$C3,(100)/(-$C3)*100)</f>
-        <v>125</v>
+        <f t="shared" ref="E3:E49" si="0">IF($C3&gt;0,$C3/100,(100)/(-$C3)+1)</f>
+        <v>4</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F49" si="2">(1/D3)</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="F3:G49" si="1">IF($C3&gt;0,$C3,(100)/(-$C3)*100)</f>
+        <v>400</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G49" si="2">IF($D3&gt;0,$D3,(100)/(-$D3)*100)</f>
+        <v>74.074074074074076</v>
+      </c>
+      <c r="H3" s="2">
+        <f>(1/E3)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -606,20 +631,24 @@
       <c r="C4">
         <v>500</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="F4" s="2">
-        <f t="shared" si="2"/>
+      <c r="G4" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="2">
+        <f>(1/E4)</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -629,20 +658,24 @@
       <c r="C5">
         <v>1200</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="F5" s="2">
-        <f t="shared" si="2"/>
+      <c r="G5" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="2">
+        <f>(1/E5)</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -650,22 +683,29 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>4000</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <v>475</v>
+      </c>
+      <c r="D6">
+        <v>-160</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
-        <v>4000</v>
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>475</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>62.5</v>
+      </c>
+      <c r="H6" s="2">
+        <f>(1/E6)</f>
+        <v>0.21052631578947367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -675,20 +715,24 @@
       <c r="C7">
         <v>2800</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>2800</v>
       </c>
-      <c r="F7" s="2">
-        <f t="shared" si="2"/>
+      <c r="G7" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="2">
+        <f>(1/E7)</f>
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -698,20 +742,24 @@
       <c r="C8">
         <v>-110</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>1.9090909090909092</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>90.909090909090907</v>
       </c>
-      <c r="F8" s="2">
-        <f t="shared" si="2"/>
+      <c r="G8" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="2">
+        <f>(1/E8)</f>
         <v>0.52380952380952384</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -721,20 +769,24 @@
       <c r="C9">
         <v>162</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>1.62</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>162</v>
       </c>
-      <c r="F9" s="2">
-        <f t="shared" si="2"/>
+      <c r="G9" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="2">
+        <f>(1/E9)</f>
         <v>0.61728395061728392</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -744,20 +796,24 @@
       <c r="C10">
         <v>700</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="F10" s="2">
-        <f t="shared" si="2"/>
+      <c r="G10" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="2">
+        <f>(1/E10)</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -765,22 +821,29 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>1400</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <v>225</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
-        <v>1400</v>
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="H11" s="2">
+        <f>(1/E11)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -790,20 +853,24 @@
       <c r="C12">
         <v>4000</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="F12" s="2">
-        <f t="shared" si="2"/>
+      <c r="G12" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="2">
+        <f>(1/E12)</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -813,20 +880,24 @@
       <c r="C13">
         <v>6600</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>6600</v>
       </c>
-      <c r="F13" s="2">
-        <f t="shared" si="2"/>
+      <c r="G13" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="2">
+        <f>(1/E13)</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -836,20 +907,24 @@
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="F14" s="2">
-        <f t="shared" si="2"/>
+      <c r="G14" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="2">
+        <f>(1/E14)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -859,20 +934,24 @@
       <c r="C15">
         <v>130</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="F15" s="2">
-        <f t="shared" si="2"/>
+      <c r="G15" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="2">
+        <f>(1/E15)</f>
         <v>0.76923076923076916</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -880,22 +959,29 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>900</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>-575</v>
+      </c>
+      <c r="D16">
+        <v>1700</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
-        <v>900</v>
+        <f t="shared" si="0"/>
+        <v>1.1739130434782608</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>17.391304347826086</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>1700</v>
+      </c>
+      <c r="H16" s="2">
+        <f>(1/E16)</f>
+        <v>0.85185185185185197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -903,22 +989,29 @@
         <v>26</v>
       </c>
       <c r="C17">
-        <v>1100</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>160</v>
+      </c>
+      <c r="D17">
+        <v>205</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>1100</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>205</v>
+      </c>
+      <c r="H17" s="2">
+        <f>(1/E17)</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -928,20 +1021,24 @@
       <c r="C18">
         <v>5000</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="F18" s="2">
-        <f t="shared" si="2"/>
+      <c r="G18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="2">
+        <f>(1/E18)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -951,20 +1048,24 @@
       <c r="C19">
         <v>6600</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>6600</v>
       </c>
-      <c r="F19" s="2">
-        <f t="shared" si="2"/>
+      <c r="G19" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="2">
+        <f>(1/E19)</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -974,20 +1075,24 @@
       <c r="C20">
         <v>-300</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="F20" s="2">
-        <f t="shared" si="2"/>
+      <c r="G20" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="2">
+        <f>(1/E20)</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -995,22 +1100,29 @@
         <v>28</v>
       </c>
       <c r="C21">
-        <v>500</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-370</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1.2702702702702702</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>27.027027027027028</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="H21" s="2">
+        <f>(1/E21)</f>
+        <v>0.78723404255319152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1020,20 +1132,24 @@
       <c r="C22">
         <v>600</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="F22" s="2">
-        <f t="shared" si="2"/>
+      <c r="G22" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="2">
+        <f>(1/E22)</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1043,20 +1159,24 @@
       <c r="C23">
         <v>1800</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <f t="shared" si="1"/>
         <v>1800</v>
       </c>
-      <c r="F23" s="2">
-        <f t="shared" si="2"/>
+      <c r="G23" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="2">
+        <f>(1/E23)</f>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1064,22 +1184,29 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>2500</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>-180</v>
+      </c>
+      <c r="D24">
+        <v>600</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="1"/>
-        <v>2500</v>
+        <f t="shared" si="0"/>
+        <v>1.5555555555555556</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="H24" s="2">
+        <f>(1/E24)</f>
+        <v>0.64285714285714279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1089,20 +1216,24 @@
       <c r="C25">
         <v>6600</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <f t="shared" si="1"/>
         <v>6600</v>
       </c>
-      <c r="F25" s="2">
-        <f t="shared" si="2"/>
+      <c r="G25" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="2">
+        <f>(1/E25)</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1112,20 +1243,24 @@
       <c r="C26">
         <v>-500</v>
       </c>
-      <c r="D26" s="2">
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F26" s="2">
-        <f t="shared" si="2"/>
+      <c r="G26" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="2">
+        <f>(1/E26)</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1135,20 +1270,24 @@
       <c r="C27">
         <v>750</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
-      <c r="F27" s="2">
-        <f t="shared" si="2"/>
+      <c r="G27" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="2">
+        <f>(1/E27)</f>
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1156,22 +1295,29 @@
         <v>14</v>
       </c>
       <c r="C28">
-        <v>1000</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-220</v>
+      </c>
+      <c r="D28">
+        <v>600</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f t="shared" si="0"/>
+        <v>1.4545454545454546</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="H28" s="2">
+        <f>(1/E28)</f>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1181,20 +1327,24 @@
       <c r="C29">
         <v>1600</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <f t="shared" si="1"/>
         <v>1600</v>
       </c>
-      <c r="F29" s="2">
-        <f t="shared" si="2"/>
+      <c r="G29" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="2">
+        <f>(1/E29)</f>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1204,20 +1354,24 @@
       <c r="C30">
         <v>2500</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="F30" s="2">
-        <f t="shared" si="2"/>
+      <c r="G30" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="2">
+        <f>(1/E30)</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1227,20 +1381,24 @@
       <c r="C31">
         <v>15000</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E31" s="2">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="F31" s="2">
-        <f t="shared" si="2"/>
+      <c r="G31" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="2">
+        <f>(1/E31)</f>
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1250,20 +1408,24 @@
       <c r="C32">
         <v>-163</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <f t="shared" si="0"/>
         <v>1.6134969325153374</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <f t="shared" si="1"/>
         <v>61.349693251533743</v>
       </c>
-      <c r="F32" s="2">
-        <f t="shared" si="2"/>
+      <c r="G32" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="2">
+        <f>(1/E32)</f>
         <v>0.61977186311787069</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1273,20 +1435,24 @@
       <c r="C33">
         <v>400</v>
       </c>
-      <c r="D33" s="2">
+      <c r="E33" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="2">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="F33" s="2">
-        <f t="shared" si="2"/>
+      <c r="G33" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="2">
+        <f>(1/E33)</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1294,22 +1460,29 @@
         <v>17</v>
       </c>
       <c r="C34">
-        <v>450</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>-195</v>
+      </c>
+      <c r="D34">
+        <v>550</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="1"/>
-        <v>450</v>
+        <f t="shared" si="0"/>
+        <v>1.5128205128205128</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="2"/>
-        <v>0.22222222222222221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>51.282051282051277</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="H34" s="2">
+        <f>(1/E34)</f>
+        <v>0.66101694915254239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1317,22 +1490,29 @@
         <v>29</v>
       </c>
       <c r="C35">
-        <v>1000</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>290</v>
+      </c>
+      <c r="D35">
+        <v>110</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f t="shared" si="0"/>
+        <v>2.9</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="H35" s="2">
+        <f>(1/E35)</f>
+        <v>0.34482758620689657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1342,20 +1522,24 @@
       <c r="C36">
         <v>1400</v>
       </c>
-      <c r="D36" s="2">
+      <c r="E36" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
-      <c r="F36" s="2">
-        <f t="shared" si="2"/>
+      <c r="G36" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="2">
+        <f>(1/E36)</f>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1365,20 +1549,24 @@
       <c r="C37">
         <v>4000</v>
       </c>
-      <c r="D37" s="2">
+      <c r="E37" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="2">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="F37" s="2">
-        <f t="shared" si="2"/>
+      <c r="G37" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="2">
+        <f>(1/E37)</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -1388,20 +1576,24 @@
       <c r="C38">
         <v>110</v>
       </c>
-      <c r="D38" s="2">
+      <c r="E38" s="2">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="2">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="F38" s="2">
-        <f t="shared" si="2"/>
+      <c r="G38" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="2">
+        <f>(1/E38)</f>
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1409,22 +1601,29 @@
         <v>19</v>
       </c>
       <c r="C39">
-        <v>137</v>
-      </c>
-      <c r="D39" s="2">
-        <f t="shared" si="0"/>
-        <v>1.37</v>
+        <v>-210</v>
+      </c>
+      <c r="D39">
+        <v>600</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="1"/>
-        <v>137</v>
+        <f t="shared" si="0"/>
+        <v>1.4761904761904763</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="2"/>
-        <v>0.72992700729927007</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>47.619047619047613</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="H39" s="2">
+        <f>(1/E39)</f>
+        <v>0.67741935483870963</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1434,20 +1633,24 @@
       <c r="C40">
         <v>500</v>
       </c>
-      <c r="D40" s="2">
+      <c r="E40" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E40" s="2">
+      <c r="F40" s="2">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="F40" s="2">
-        <f t="shared" si="2"/>
+      <c r="G40" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="2">
+        <f>(1/E40)</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1457,20 +1660,24 @@
       <c r="C41">
         <v>1400</v>
       </c>
-      <c r="D41" s="2">
+      <c r="E41" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="2">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
-      <c r="F41" s="2">
-        <f t="shared" si="2"/>
+      <c r="G41" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="2">
+        <f>(1/E41)</f>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1478,22 +1685,29 @@
         <v>30</v>
       </c>
       <c r="C42">
-        <v>4000</v>
-      </c>
-      <c r="D42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <v>-130</v>
+      </c>
+      <c r="D42">
+        <v>400</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="1"/>
-        <v>4000</v>
+        <f t="shared" si="0"/>
+        <v>1.7692307692307692</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>76.923076923076934</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="H42" s="2">
+        <f>(1/E42)</f>
+        <v>0.56521739130434789</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1503,20 +1717,24 @@
       <c r="C43">
         <v>5000</v>
       </c>
-      <c r="D43" s="2">
+      <c r="E43" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="2">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="F43" s="2">
-        <f t="shared" si="2"/>
+      <c r="G43" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="2">
+        <f>(1/E43)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1526,20 +1744,24 @@
       <c r="C44">
         <v>-175</v>
       </c>
-      <c r="D44" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="0"/>
         <v>1.5714285714285714</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="2">
         <f t="shared" si="1"/>
         <v>57.142857142857139</v>
       </c>
-      <c r="F44" s="2">
-        <f t="shared" si="2"/>
+      <c r="G44" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" s="2">
+        <f>(1/E44)</f>
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1547,22 +1769,29 @@
         <v>22</v>
       </c>
       <c r="C45">
-        <v>500</v>
-      </c>
-      <c r="D45" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-270</v>
+      </c>
+      <c r="D45">
+        <v>850</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1.3703703703703702</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="2"/>
+        <v>850</v>
+      </c>
+      <c r="H45" s="2">
+        <f>(1/E45)</f>
+        <v>0.72972972972972983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1572,20 +1801,24 @@
       <c r="C46">
         <v>400</v>
       </c>
-      <c r="D46" s="2">
+      <c r="E46" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E46" s="2">
+      <c r="F46" s="2">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="F46" s="2">
-        <f t="shared" si="2"/>
+      <c r="G46" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" s="2">
+        <f>(1/E46)</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -1595,20 +1828,24 @@
       <c r="C47">
         <v>1600</v>
       </c>
-      <c r="D47" s="2">
+      <c r="E47" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E47" s="2">
+      <c r="F47" s="2">
         <f t="shared" si="1"/>
         <v>1600</v>
       </c>
-      <c r="F47" s="2">
-        <f t="shared" si="2"/>
+      <c r="G47" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" s="2">
+        <f>(1/E47)</f>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1616,22 +1853,29 @@
         <v>32</v>
       </c>
       <c r="C48">
-        <v>1400</v>
-      </c>
-      <c r="D48" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>-135</v>
+      </c>
+      <c r="D48">
+        <v>425</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="1"/>
-        <v>1400</v>
+        <f t="shared" si="0"/>
+        <v>1.7407407407407407</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="1"/>
+        <v>74.074074074074076</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="2"/>
+        <v>425</v>
+      </c>
+      <c r="H48" s="2">
+        <f>(1/E48)</f>
+        <v>0.57446808510638303</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -1641,16 +1885,20 @@
       <c r="C49">
         <v>6600</v>
       </c>
-      <c r="D49" s="2">
+      <c r="E49" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="E49" s="2">
+      <c r="F49" s="2">
         <f t="shared" si="1"/>
         <v>6600</v>
       </c>
-      <c r="F49" s="2">
-        <f t="shared" si="2"/>
+      <c r="G49" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H49" s="2">
+        <f>(1/E49)</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>

</xml_diff>